<commit_message>
Add data driven test
</commit_message>
<xml_diff>
--- a/05-data-driven-framework/Data/HomepageData.xlsx
+++ b/05-data-driven-framework/Data/HomepageData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panchava-1\OneDrive - Mettler Toledo LLC\Backup\General\Projects\Automation\selenium-csharp\05-data-driven-framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF731263-973F-429C-BFBA-89498E23FCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616913A3-6A5A-4690-A9BE-69E90D1C4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -36,10 +36,16 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Gopalakrishnan</t>
-  </si>
-  <si>
-    <t>gopalakrishnan1505@gmail.com</t>
+    <t>UserOne</t>
+  </si>
+  <si>
+    <t>UserTwo</t>
+  </si>
+  <si>
+    <t>testuserone@gmail.com</t>
+  </si>
+  <si>
+    <t>testusertwo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -373,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -402,15 +408,27 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E6669D0F-5A71-4EE3-B270-50B8300DD051}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{051A245F-5294-48A4-8AFF-C4E3F066D8B5}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A79F85E2-CB5A-4DC1-AB63-C9FE96AD47AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete Excel Data read
</commit_message>
<xml_diff>
--- a/05-data-driven-framework/Data/HomepageData.xlsx
+++ b/05-data-driven-framework/Data/HomepageData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panchava-1\OneDrive - Mettler Toledo LLC\Backup\General\Projects\Automation\selenium-csharp\05-data-driven-framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616913A3-6A5A-4690-A9BE-69E90D1C4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFDBB67-FC4F-4AD4-AB27-B57CB6AEA238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,16 @@
     <t>Email</t>
   </si>
   <si>
-    <t>UserOne</t>
-  </si>
-  <si>
-    <t>UserTwo</t>
-  </si>
-  <si>
-    <t>testuserone@gmail.com</t>
-  </si>
-  <si>
-    <t>testusertwo@gmail.com</t>
+    <t>testuser@test.com</t>
+  </si>
+  <si>
+    <t>Gopal</t>
+  </si>
+  <si>
+    <t>TestUser</t>
+  </si>
+  <si>
+    <t>testuser2@test.com</t>
   </si>
 </sst>
 </file>
@@ -69,15 +69,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,19 +91,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -382,14 +407,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="28.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -404,31 +427,31 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{051A245F-5294-48A4-8AFF-C4E3F066D8B5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{A79F85E2-CB5A-4DC1-AB63-C9FE96AD47AD}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{712783E3-3117-47CA-A6E2-37C974224B38}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{DA3E3F3A-2376-4111-8BBF-1E0688537D44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>